<commit_message>
added data for course categories and compulsory courses
</commit_message>
<xml_diff>
--- a/Raw Data/Course Enrollment Numbers.xlsx
+++ b/Raw Data/Course Enrollment Numbers.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="M:\TAOR\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uoe-my.sharepoint.com/personal/s1941220_ed_ac_uk/Documents/Year 5/SEM2/Topics in Applied OR/taor_project/taor_project/Raw Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C6B764E2-8ABC-4168-BFD5-5A57A68EA1B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="187" documentId="8_{C6B764E2-8ABC-4168-BFD5-5A57A68EA1B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BAD7318E-100E-428A-90B2-1672E169A5FD}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Course Numbers" sheetId="2" r:id="rId1"/>
+    <sheet name="categories and compulsory" sheetId="4" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="481" uniqueCount="235">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1095" uniqueCount="289">
   <si>
     <t>Delivery Period</t>
   </si>
@@ -741,16 +742,182 @@
   </si>
   <si>
     <t>Numerical Methods for Data</t>
+  </si>
+  <si>
+    <t>Categories</t>
+  </si>
+  <si>
+    <t>Data Science, Statistics</t>
+  </si>
+  <si>
+    <t>Applied &amp; Computational</t>
+  </si>
+  <si>
+    <t>Data Science, Optimization &amp; Operational Research</t>
+  </si>
+  <si>
+    <t>Probability, Statistics</t>
+  </si>
+  <si>
+    <t>Financial</t>
+  </si>
+  <si>
+    <t>Analysis</t>
+  </si>
+  <si>
+    <t>Algebra</t>
+  </si>
+  <si>
+    <t>Financial, Probability</t>
+  </si>
+  <si>
+    <t>Statistics</t>
+  </si>
+  <si>
+    <t>Analysis, Probability</t>
+  </si>
+  <si>
+    <t>Optimization &amp; Operational Research</t>
+  </si>
+  <si>
+    <t>Geometry &amp; Topology</t>
+  </si>
+  <si>
+    <t>Algebra, Geometry &amp; Topology</t>
+  </si>
+  <si>
+    <t>Applied &amp; Computational, Data Science, Optimization &amp; Operational Research</t>
+  </si>
+  <si>
+    <t>Optimization &amp; Operational Research, Probability, Statistics</t>
+  </si>
+  <si>
+    <t>Geometry &amp; Topology, Mathematical Physics</t>
+  </si>
+  <si>
+    <t>Financial, Statistics</t>
+  </si>
+  <si>
+    <t>Financial, Optimization &amp; Operational Research</t>
+  </si>
+  <si>
+    <t>Mathematical Physics</t>
+  </si>
+  <si>
+    <t>Applied &amp; Computational, Data Science</t>
+  </si>
+  <si>
+    <t>Applied &amp; Computational, Data Science, Statistics</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Financial </t>
+  </si>
+  <si>
+    <t>Degrees Compulsory For</t>
+  </si>
+  <si>
+    <t>ambsc, ammmath, mbsc, mma, mmmath, mnst, mnbu</t>
+  </si>
+  <si>
+    <t>ambsc, ammmath, mbsc, mma, mmmath, mnbu, mnmu, mnph, mnst</t>
+  </si>
+  <si>
+    <t>ambsc, ammmath, mbsc, mma, mmmath, mnbu, mnmu, mnst</t>
+  </si>
+  <si>
+    <t>ambsc, ammmath, mbsc, mma, mmmath, mnbu, mnst</t>
+  </si>
+  <si>
+    <t>ambsc, ammmath, mbsc, mma, mmmath, mnbu, mnph, mnst</t>
+  </si>
+  <si>
+    <t>mbsc, mnbu, mnst</t>
+  </si>
+  <si>
+    <t>ambsc, ammmath, mbsc, mma, mnph, mnst</t>
+  </si>
+  <si>
+    <t>mnbi</t>
+  </si>
+  <si>
+    <t>ambsc, ammmath, mnbi</t>
+  </si>
+  <si>
+    <t>ambsc, ammmath, mbsc, mma, mmmath, mnbi, mnbi, mnph</t>
+  </si>
+  <si>
+    <t>ambsc, ammmath, mbsc, mma, mmmath, mnbi, mnbu, mnph</t>
+  </si>
+  <si>
+    <t>ambsc, ammmath, mbsc, mma, mmmath</t>
+  </si>
+  <si>
+    <t>ammmath, mbsc, mma, mmmath</t>
+  </si>
+  <si>
+    <t>mnst</t>
+  </si>
+  <si>
+    <t>mnbi, mnst</t>
+  </si>
+  <si>
+    <t>ambsc, ammmath, cammsc</t>
+  </si>
+  <si>
+    <t>ords, orco, orwr, ormsc, storft, storpt</t>
+  </si>
+  <si>
+    <t>orco, orwr, ormsc, storft, storpt</t>
+  </si>
+  <si>
+    <t>orco, orwr, ormsc</t>
+  </si>
+  <si>
+    <t>cammsc</t>
+  </si>
+  <si>
+    <t>cmfft, cmfpt, fmoft, fmopt</t>
+  </si>
+  <si>
+    <t>cmfft, cmfpt</t>
+  </si>
+  <si>
+    <t>fmoft, fmopt</t>
+  </si>
+  <si>
+    <t>stds</t>
+  </si>
+  <si>
+    <t>storft, storpt</t>
+  </si>
+  <si>
+    <t>stds, storft, storpt</t>
+  </si>
+  <si>
+    <t>ammmath</t>
+  </si>
+  <si>
+    <t>cmfft, cmfpt, cammsc</t>
+  </si>
+  <si>
+    <t>ammmath, cammsc</t>
+  </si>
+  <si>
+    <t>fmoft, fmopt, ords, orco, orwr, ormsc, storft, storpt</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Arial"/>
     </font>
   </fonts>
@@ -778,7 +945,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -793,6 +960,10 @@
 </styleSheet>
 </file>
 
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{DF92AE52-9B88-4AB0-B44F-42B61BC36B3E}" name="Table1" displayName="Table1" ref="A1:G110" totalsRowShown="0">
   <autoFilter ref="A1:G110" xr:uid="{DF92AE52-9B88-4AB0-B44F-42B61BC36B3E}"/>
@@ -804,6 +975,24 @@
     <tableColumn id="7" xr3:uid="{E6D6369B-0E1F-4E97-9260-C7AC64B967F5}" name="20/21"/>
     <tableColumn id="8" xr3:uid="{F3F9D2B4-7F53-43CA-AB9A-CE04DE183713}" name="21/22"/>
     <tableColumn id="9" xr3:uid="{E5586218-B39B-4214-B58C-362364AEE64B}" name="22/23"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{3762586E-5C99-4EBE-B29F-9EF2D4FC98EE}" name="Table13" displayName="Table13" ref="A1:I110" totalsRowShown="0">
+  <autoFilter ref="A1:I110" xr:uid="{3762586E-5C99-4EBE-B29F-9EF2D4FC98EE}"/>
+  <tableColumns count="9">
+    <tableColumn id="1" xr3:uid="{4AB2DF69-EA3D-45E1-B0A9-C42801BB1737}" name="Delivery Period"/>
+    <tableColumn id="2" xr3:uid="{357881A7-E338-42D9-B569-82E1281B8D0B}" name="Normal Year Taken"/>
+    <tableColumn id="3" xr3:uid="{4F1621C7-00C6-4600-BA81-EAE4C8DF1F96}" name="Code"/>
+    <tableColumn id="4" xr3:uid="{D8C976B4-1FFD-4BD4-9FF8-5752A0A3A803}" name="Course"/>
+    <tableColumn id="7" xr3:uid="{9A75A38A-DAA0-4197-864E-7A035329FB1B}" name="20/21"/>
+    <tableColumn id="8" xr3:uid="{9C4294C5-BFAE-45F7-831C-79314BC4298A}" name="21/22"/>
+    <tableColumn id="9" xr3:uid="{91ADC1DC-7DA7-4828-9484-569078BC0BD4}" name="22/23"/>
+    <tableColumn id="5" xr3:uid="{BE209AEC-96D4-4F60-B0A6-AE9B92EB4B43}" name="Categories"/>
+    <tableColumn id="6" xr3:uid="{FF0E3CF3-0ADE-4366-AD45-0C929AE2D069}" name="Degrees Compulsory For"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1108,20 +1297,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A822037E-5C52-4B8E-9B3D-ADEBD13DC762}">
   <dimension ref="A1:G110"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P35" sqref="P35"/>
+    <sheetView topLeftCell="A81" workbookViewId="0">
+      <selection sqref="A1:G110"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.44140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="21" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="50.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="7" width="7.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="50.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="7" width="7.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1144,7 +1333,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -1167,7 +1356,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -1190,7 +1379,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>13</v>
       </c>
@@ -1213,7 +1402,7 @@
         <v>396</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -1236,7 +1425,7 @@
         <v>560</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>13</v>
       </c>
@@ -1259,7 +1448,7 @@
         <v>590</v>
       </c>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>13</v>
       </c>
@@ -1282,7 +1471,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -1305,7 +1494,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -1328,7 +1517,7 @@
         <v>448</v>
       </c>
     </row>
-    <row r="10" spans="1:7">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>13</v>
       </c>
@@ -1351,7 +1540,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="11" spans="1:7">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>13</v>
       </c>
@@ -1374,7 +1563,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="12" spans="1:7">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>7</v>
       </c>
@@ -1397,7 +1586,7 @@
         <v>455</v>
       </c>
     </row>
-    <row r="13" spans="1:7">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>7</v>
       </c>
@@ -1420,7 +1609,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="14" spans="1:7">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>7</v>
       </c>
@@ -1443,7 +1632,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="15" spans="1:7">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>7</v>
       </c>
@@ -1466,7 +1655,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="16" spans="1:7">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>13</v>
       </c>
@@ -1489,7 +1678,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="17" spans="1:7">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>7</v>
       </c>
@@ -1512,7 +1701,7 @@
         <v>403</v>
       </c>
     </row>
-    <row r="18" spans="1:7">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>13</v>
       </c>
@@ -1535,7 +1724,7 @@
         <v>410</v>
       </c>
     </row>
-    <row r="19" spans="1:7">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>7</v>
       </c>
@@ -1558,7 +1747,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="20" spans="1:7">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>13</v>
       </c>
@@ -1581,7 +1770,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="21" spans="1:7">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>7</v>
       </c>
@@ -1604,7 +1793,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="22" spans="1:7">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>52</v>
       </c>
@@ -1627,7 +1816,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="23" spans="1:7">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>7</v>
       </c>
@@ -1650,7 +1839,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="24" spans="1:7">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>13</v>
       </c>
@@ -1673,7 +1862,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="25" spans="1:7">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>7</v>
       </c>
@@ -1696,7 +1885,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="26" spans="1:7">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>52</v>
       </c>
@@ -1719,7 +1908,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="27" spans="1:7">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>7</v>
       </c>
@@ -1742,7 +1931,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="28" spans="1:7">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>7</v>
       </c>
@@ -1765,7 +1954,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="29" spans="1:7">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>13</v>
       </c>
@@ -1788,7 +1977,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="30" spans="1:7">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>7</v>
       </c>
@@ -1811,7 +2000,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="31" spans="1:7">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>13</v>
       </c>
@@ -1834,7 +2023,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="32" spans="1:7">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>13</v>
       </c>
@@ -1857,7 +2046,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="33" spans="1:7">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>7</v>
       </c>
@@ -1880,7 +2069,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="34" spans="1:7">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>7</v>
       </c>
@@ -1903,7 +2092,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="35" spans="1:7">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>13</v>
       </c>
@@ -1926,7 +2115,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="36" spans="1:7">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>7</v>
       </c>
@@ -1949,7 +2138,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="37" spans="1:7">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>13</v>
       </c>
@@ -1972,7 +2161,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="38" spans="1:7">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>13</v>
       </c>
@@ -1995,7 +2184,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="39" spans="1:7">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>7</v>
       </c>
@@ -2018,7 +2207,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="40" spans="1:7">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>13</v>
       </c>
@@ -2041,7 +2230,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="41" spans="1:7">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>7</v>
       </c>
@@ -2064,7 +2253,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="42" spans="1:7">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>7</v>
       </c>
@@ -2087,7 +2276,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="43" spans="1:7">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>13</v>
       </c>
@@ -2110,7 +2299,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="44" spans="1:7">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>7</v>
       </c>
@@ -2133,7 +2322,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="45" spans="1:7">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>13</v>
       </c>
@@ -2156,7 +2345,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="46" spans="1:7">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>7</v>
       </c>
@@ -2179,7 +2368,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="47" spans="1:7">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>13</v>
       </c>
@@ -2202,7 +2391,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="48" spans="1:7">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>13</v>
       </c>
@@ -2225,7 +2414,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="49" spans="1:7">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>13</v>
       </c>
@@ -2248,7 +2437,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="50" spans="1:7">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>7</v>
       </c>
@@ -2271,7 +2460,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="51" spans="1:7">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>7</v>
       </c>
@@ -2294,7 +2483,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="52" spans="1:7">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>7</v>
       </c>
@@ -2317,7 +2506,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="53" spans="1:7">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>7</v>
       </c>
@@ -2340,7 +2529,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="54" spans="1:7">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>13</v>
       </c>
@@ -2363,7 +2552,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="55" spans="1:7">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>52</v>
       </c>
@@ -2386,7 +2575,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="56" spans="1:7">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>7</v>
       </c>
@@ -2409,7 +2598,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="57" spans="1:7">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>13</v>
       </c>
@@ -2432,7 +2621,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="58" spans="1:7">
+    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>7</v>
       </c>
@@ -2455,7 +2644,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="59" spans="1:7">
+    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>7</v>
       </c>
@@ -2478,7 +2667,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="60" spans="1:7">
+    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>7</v>
       </c>
@@ -2501,7 +2690,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="61" spans="1:7">
+    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>7</v>
       </c>
@@ -2524,7 +2713,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="62" spans="1:7">
+    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>13</v>
       </c>
@@ -2547,7 +2736,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="63" spans="1:7">
+    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>13</v>
       </c>
@@ -2570,7 +2759,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="64" spans="1:7">
+    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>13</v>
       </c>
@@ -2593,7 +2782,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="65" spans="1:7">
+    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>13</v>
       </c>
@@ -2616,7 +2805,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="66" spans="1:7">
+    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>13</v>
       </c>
@@ -2639,7 +2828,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="67" spans="1:7">
+    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>7</v>
       </c>
@@ -2662,7 +2851,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="68" spans="1:7">
+    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>13</v>
       </c>
@@ -2685,7 +2874,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="69" spans="1:7">
+    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>13</v>
       </c>
@@ -2708,7 +2897,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="70" spans="1:7">
+    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>13</v>
       </c>
@@ -2731,7 +2920,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="71" spans="1:7">
+    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>13</v>
       </c>
@@ -2754,7 +2943,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="72" spans="1:7">
+    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>13</v>
       </c>
@@ -2777,7 +2966,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="73" spans="1:7">
+    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>7</v>
       </c>
@@ -2800,7 +2989,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="74" spans="1:7">
+    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>7</v>
       </c>
@@ -2823,7 +3012,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="75" spans="1:7">
+    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>13</v>
       </c>
@@ -2846,7 +3035,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="76" spans="1:7">
+    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>13</v>
       </c>
@@ -2869,7 +3058,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="77" spans="1:7">
+    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>13</v>
       </c>
@@ -2892,7 +3081,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="78" spans="1:7">
+    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>13</v>
       </c>
@@ -2915,7 +3104,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="79" spans="1:7">
+    <row r="79" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>7</v>
       </c>
@@ -2938,7 +3127,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="80" spans="1:7">
+    <row r="80" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>7</v>
       </c>
@@ -2961,7 +3150,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="81" spans="1:7">
+    <row r="81" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>7</v>
       </c>
@@ -2984,7 +3173,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="82" spans="1:7">
+    <row r="82" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>7</v>
       </c>
@@ -3007,7 +3196,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="83" spans="1:7">
+    <row r="83" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>13</v>
       </c>
@@ -3030,7 +3219,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="84" spans="1:7">
+    <row r="84" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>13</v>
       </c>
@@ -3053,7 +3242,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="85" spans="1:7">
+    <row r="85" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>13</v>
       </c>
@@ -3076,7 +3265,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="86" spans="1:7">
+    <row r="86" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>13</v>
       </c>
@@ -3099,7 +3288,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="87" spans="1:7">
+    <row r="87" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>7</v>
       </c>
@@ -3122,7 +3311,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="88" spans="1:7">
+    <row r="88" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>13</v>
       </c>
@@ -3145,7 +3334,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="89" spans="1:7">
+    <row r="89" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>13</v>
       </c>
@@ -3168,7 +3357,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="90" spans="1:7">
+    <row r="90" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>13</v>
       </c>
@@ -3191,7 +3380,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="91" spans="1:7">
+    <row r="91" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>13</v>
       </c>
@@ -3214,7 +3403,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="92" spans="1:7">
+    <row r="92" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>52</v>
       </c>
@@ -3237,7 +3426,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="93" spans="1:7">
+    <row r="93" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>7</v>
       </c>
@@ -3260,7 +3449,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="94" spans="1:7">
+    <row r="94" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>13</v>
       </c>
@@ -3283,7 +3472,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="95" spans="1:7">
+    <row r="95" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>7</v>
       </c>
@@ -3306,7 +3495,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="96" spans="1:7">
+    <row r="96" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>13</v>
       </c>
@@ -3329,7 +3518,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="97" spans="1:7">
+    <row r="97" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>13</v>
       </c>
@@ -3352,7 +3541,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="98" spans="1:7">
+    <row r="98" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>13</v>
       </c>
@@ -3375,7 +3564,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="99" spans="1:7">
+    <row r="99" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>13</v>
       </c>
@@ -3398,7 +3587,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="100" spans="1:7">
+    <row r="100" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>7</v>
       </c>
@@ -3421,7 +3610,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="101" spans="1:7">
+    <row r="101" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>13</v>
       </c>
@@ -3444,7 +3633,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="102" spans="1:7">
+    <row r="102" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>13</v>
       </c>
@@ -3467,7 +3656,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="103" spans="1:7">
+    <row r="103" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>13</v>
       </c>
@@ -3490,7 +3679,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="104" spans="1:7">
+    <row r="104" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>7</v>
       </c>
@@ -3513,7 +3702,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="105" spans="1:7">
+    <row r="105" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>7</v>
       </c>
@@ -3536,7 +3725,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="106" spans="1:7">
+    <row r="106" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>13</v>
       </c>
@@ -3559,7 +3748,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="107" spans="1:7">
+    <row r="107" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>7</v>
       </c>
@@ -3582,7 +3771,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="108" spans="1:7">
+    <row r="108" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>7</v>
       </c>
@@ -3605,7 +3794,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="109" spans="1:7">
+    <row r="109" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>13</v>
       </c>
@@ -3628,7 +3817,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="110" spans="1:7">
+    <row r="110" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>13</v>
       </c>
@@ -3659,16 +3848,2964 @@
 </worksheet>
 </file>
 
-<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A58DA5D3-B845-41C8-B44B-BDBE695086ED}">
+  <dimension ref="A1:I110"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I61" sqref="I61"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="28.77734375" customWidth="1"/>
+    <col min="5" max="7" width="7.77734375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="37.6640625" customWidth="1"/>
+    <col min="9" max="9" width="56.77734375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>235</v>
+      </c>
+      <c r="I1" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2">
+        <v>171</v>
+      </c>
+      <c r="F2">
+        <v>273</v>
+      </c>
+      <c r="G2">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3">
+        <v>14</v>
+      </c>
+      <c r="F3">
+        <v>36</v>
+      </c>
+      <c r="G3">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D4" t="s">
+        <v>16</v>
+      </c>
+      <c r="E4">
+        <v>302</v>
+      </c>
+      <c r="F4">
+        <v>327</v>
+      </c>
+      <c r="G4">
+        <v>396</v>
+      </c>
+      <c r="H4" t="s">
+        <v>236</v>
+      </c>
+      <c r="I4" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D5" t="s">
+        <v>18</v>
+      </c>
+      <c r="E5">
+        <v>682</v>
+      </c>
+      <c r="F5">
+        <v>800</v>
+      </c>
+      <c r="G5">
+        <v>560</v>
+      </c>
+      <c r="I5" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" t="s">
+        <v>19</v>
+      </c>
+      <c r="D6" t="s">
+        <v>20</v>
+      </c>
+      <c r="E6">
+        <v>708</v>
+      </c>
+      <c r="F6">
+        <v>801</v>
+      </c>
+      <c r="G6">
+        <v>590</v>
+      </c>
+      <c r="I6" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D7" t="s">
+        <v>22</v>
+      </c>
+      <c r="E7">
+        <v>435</v>
+      </c>
+      <c r="F7">
+        <v>517</v>
+      </c>
+      <c r="G7">
+        <v>376</v>
+      </c>
+      <c r="I7" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>14</v>
+      </c>
+      <c r="C8" t="s">
+        <v>23</v>
+      </c>
+      <c r="D8" t="s">
+        <v>24</v>
+      </c>
+      <c r="E8">
+        <v>58</v>
+      </c>
+      <c r="F8">
+        <v>63</v>
+      </c>
+      <c r="G8">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" t="s">
+        <v>14</v>
+      </c>
+      <c r="C9" t="s">
+        <v>25</v>
+      </c>
+      <c r="D9" t="s">
+        <v>26</v>
+      </c>
+      <c r="E9">
+        <v>373</v>
+      </c>
+      <c r="F9">
+        <v>411</v>
+      </c>
+      <c r="G9">
+        <v>448</v>
+      </c>
+      <c r="H9" t="s">
+        <v>237</v>
+      </c>
+      <c r="I9" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>13</v>
+      </c>
+      <c r="B10" t="s">
+        <v>14</v>
+      </c>
+      <c r="C10" t="s">
+        <v>27</v>
+      </c>
+      <c r="D10" t="s">
+        <v>28</v>
+      </c>
+      <c r="E10">
+        <v>355</v>
+      </c>
+      <c r="F10">
+        <v>391</v>
+      </c>
+      <c r="G10">
+        <v>461</v>
+      </c>
+      <c r="H10" t="s">
+        <v>238</v>
+      </c>
+      <c r="I10" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>13</v>
+      </c>
+      <c r="B11" t="s">
+        <v>14</v>
+      </c>
+      <c r="C11" t="s">
+        <v>29</v>
+      </c>
+      <c r="D11" t="s">
+        <v>30</v>
+      </c>
+      <c r="E11">
+        <v>247</v>
+      </c>
+      <c r="F11">
+        <v>296</v>
+      </c>
+      <c r="G11">
+        <v>386</v>
+      </c>
+      <c r="H11" t="s">
+        <v>237</v>
+      </c>
+      <c r="I11" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>7</v>
+      </c>
+      <c r="B12" t="s">
+        <v>14</v>
+      </c>
+      <c r="C12" t="s">
+        <v>31</v>
+      </c>
+      <c r="D12" t="s">
+        <v>32</v>
+      </c>
+      <c r="E12">
+        <v>353</v>
+      </c>
+      <c r="F12">
+        <v>388</v>
+      </c>
+      <c r="G12">
+        <v>455</v>
+      </c>
+      <c r="H12" t="s">
+        <v>239</v>
+      </c>
+      <c r="I12" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>7</v>
+      </c>
+      <c r="B13" t="s">
+        <v>14</v>
+      </c>
+      <c r="C13" t="s">
+        <v>33</v>
+      </c>
+      <c r="D13" t="s">
+        <v>34</v>
+      </c>
+      <c r="E13">
+        <v>156</v>
+      </c>
+      <c r="F13">
+        <v>184</v>
+      </c>
+      <c r="G13">
+        <v>274</v>
+      </c>
+      <c r="I13" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>7</v>
+      </c>
+      <c r="B14" t="s">
+        <v>14</v>
+      </c>
+      <c r="C14" t="s">
+        <v>35</v>
+      </c>
+      <c r="D14" t="s">
+        <v>36</v>
+      </c>
+      <c r="E14">
+        <v>81</v>
+      </c>
+      <c r="F14">
+        <v>76</v>
+      </c>
+      <c r="G14">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>7</v>
+      </c>
+      <c r="B15" t="s">
+        <v>8</v>
+      </c>
+      <c r="C15" t="s">
+        <v>37</v>
+      </c>
+      <c r="D15" t="s">
+        <v>38</v>
+      </c>
+      <c r="E15">
+        <v>120</v>
+      </c>
+      <c r="F15">
+        <v>82</v>
+      </c>
+      <c r="G15">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>13</v>
+      </c>
+      <c r="B16" t="s">
+        <v>8</v>
+      </c>
+      <c r="C16" t="s">
+        <v>39</v>
+      </c>
+      <c r="D16" t="s">
+        <v>40</v>
+      </c>
+      <c r="E16">
+        <v>114</v>
+      </c>
+      <c r="F16">
+        <v>84</v>
+      </c>
+      <c r="G16">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>7</v>
+      </c>
+      <c r="B17" t="s">
+        <v>8</v>
+      </c>
+      <c r="C17" t="s">
+        <v>41</v>
+      </c>
+      <c r="D17" t="s">
+        <v>42</v>
+      </c>
+      <c r="E17">
+        <v>352</v>
+      </c>
+      <c r="F17">
+        <v>394</v>
+      </c>
+      <c r="G17">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>13</v>
+      </c>
+      <c r="B18" t="s">
+        <v>8</v>
+      </c>
+      <c r="C18" t="s">
+        <v>43</v>
+      </c>
+      <c r="D18" t="s">
+        <v>44</v>
+      </c>
+      <c r="E18">
+        <v>386</v>
+      </c>
+      <c r="F18">
+        <v>394</v>
+      </c>
+      <c r="G18">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>7</v>
+      </c>
+      <c r="B19" t="s">
+        <v>8</v>
+      </c>
+      <c r="C19" t="s">
+        <v>45</v>
+      </c>
+      <c r="D19" t="s">
+        <v>46</v>
+      </c>
+      <c r="E19">
+        <v>244</v>
+      </c>
+      <c r="F19">
+        <v>318</v>
+      </c>
+      <c r="G19">
+        <v>173</v>
+      </c>
+      <c r="H19" t="s">
+        <v>236</v>
+      </c>
+      <c r="I19" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>13</v>
+      </c>
+      <c r="B20" t="s">
+        <v>47</v>
+      </c>
+      <c r="C20" t="s">
+        <v>48</v>
+      </c>
+      <c r="D20" t="s">
+        <v>49</v>
+      </c>
+      <c r="E20">
+        <v>176</v>
+      </c>
+      <c r="F20">
+        <v>167</v>
+      </c>
+      <c r="G20">
+        <v>197</v>
+      </c>
+      <c r="H20" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>7</v>
+      </c>
+      <c r="B21" t="s">
+        <v>47</v>
+      </c>
+      <c r="C21" t="s">
+        <v>50</v>
+      </c>
+      <c r="D21" t="s">
+        <v>51</v>
+      </c>
+      <c r="E21">
+        <v>171</v>
+      </c>
+      <c r="F21">
+        <v>151</v>
+      </c>
+      <c r="G21">
+        <v>149</v>
+      </c>
+      <c r="H21" t="s">
+        <v>239</v>
+      </c>
+      <c r="I21" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>52</v>
+      </c>
+      <c r="B22" t="s">
+        <v>53</v>
+      </c>
+      <c r="C22" t="s">
+        <v>54</v>
+      </c>
+      <c r="D22" t="s">
+        <v>55</v>
+      </c>
+      <c r="E22">
+        <v>52</v>
+      </c>
+      <c r="F22">
+        <v>52</v>
+      </c>
+      <c r="G22">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>7</v>
+      </c>
+      <c r="B23" t="s">
+        <v>53</v>
+      </c>
+      <c r="C23" t="s">
+        <v>56</v>
+      </c>
+      <c r="D23" t="s">
+        <v>57</v>
+      </c>
+      <c r="E23">
+        <v>29</v>
+      </c>
+      <c r="F23">
+        <v>35</v>
+      </c>
+      <c r="G23">
+        <v>62</v>
+      </c>
+      <c r="H23" t="s">
+        <v>237</v>
+      </c>
+      <c r="I23" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>13</v>
+      </c>
+      <c r="B24" t="s">
+        <v>58</v>
+      </c>
+      <c r="C24" t="s">
+        <v>59</v>
+      </c>
+      <c r="D24" t="s">
+        <v>60</v>
+      </c>
+      <c r="E24" t="s">
+        <v>61</v>
+      </c>
+      <c r="F24">
+        <v>20</v>
+      </c>
+      <c r="G24" t="s">
+        <v>61</v>
+      </c>
+      <c r="H24" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>7</v>
+      </c>
+      <c r="B25" t="s">
+        <v>53</v>
+      </c>
+      <c r="C25" t="s">
+        <v>62</v>
+      </c>
+      <c r="D25" t="s">
+        <v>63</v>
+      </c>
+      <c r="E25" t="s">
+        <v>61</v>
+      </c>
+      <c r="F25" t="s">
+        <v>61</v>
+      </c>
+      <c r="G25">
+        <v>31</v>
+      </c>
+      <c r="H25" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>52</v>
+      </c>
+      <c r="B26" t="s">
+        <v>53</v>
+      </c>
+      <c r="C26" t="s">
+        <v>64</v>
+      </c>
+      <c r="D26" t="s">
+        <v>65</v>
+      </c>
+      <c r="E26">
+        <v>29</v>
+      </c>
+      <c r="F26">
+        <v>38</v>
+      </c>
+      <c r="G26">
+        <v>7</v>
+      </c>
+      <c r="H26" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>7</v>
+      </c>
+      <c r="B27" t="s">
+        <v>53</v>
+      </c>
+      <c r="C27" t="s">
+        <v>66</v>
+      </c>
+      <c r="D27" t="s">
+        <v>67</v>
+      </c>
+      <c r="E27" t="s">
+        <v>61</v>
+      </c>
+      <c r="F27">
+        <v>51</v>
+      </c>
+      <c r="G27">
+        <v>58</v>
+      </c>
+      <c r="H27" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>7</v>
+      </c>
+      <c r="B28" t="s">
+        <v>53</v>
+      </c>
+      <c r="C28" t="s">
+        <v>68</v>
+      </c>
+      <c r="D28" t="s">
+        <v>69</v>
+      </c>
+      <c r="E28">
+        <v>25</v>
+      </c>
+      <c r="F28">
+        <v>30</v>
+      </c>
+      <c r="G28">
+        <v>26</v>
+      </c>
+      <c r="H28" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>13</v>
+      </c>
+      <c r="B29" t="s">
+        <v>53</v>
+      </c>
+      <c r="C29" t="s">
+        <v>70</v>
+      </c>
+      <c r="D29" t="s">
+        <v>71</v>
+      </c>
+      <c r="E29">
+        <v>27</v>
+      </c>
+      <c r="F29">
+        <v>35</v>
+      </c>
+      <c r="G29">
+        <v>20</v>
+      </c>
+      <c r="H29" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>7</v>
+      </c>
+      <c r="B30" t="s">
+        <v>53</v>
+      </c>
+      <c r="C30" t="s">
+        <v>72</v>
+      </c>
+      <c r="D30" t="s">
+        <v>73</v>
+      </c>
+      <c r="E30">
+        <v>65</v>
+      </c>
+      <c r="F30">
+        <v>78</v>
+      </c>
+      <c r="G30">
+        <v>52</v>
+      </c>
+      <c r="H30" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>13</v>
+      </c>
+      <c r="B31" t="s">
+        <v>47</v>
+      </c>
+      <c r="C31" t="s">
+        <v>74</v>
+      </c>
+      <c r="D31" t="s">
+        <v>75</v>
+      </c>
+      <c r="E31">
+        <v>128</v>
+      </c>
+      <c r="F31">
+        <v>145</v>
+      </c>
+      <c r="G31">
+        <v>191</v>
+      </c>
+      <c r="H31" t="s">
+        <v>237</v>
+      </c>
+      <c r="I31" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>13</v>
+      </c>
+      <c r="B32" t="s">
+        <v>53</v>
+      </c>
+      <c r="C32" t="s">
+        <v>76</v>
+      </c>
+      <c r="D32" t="s">
+        <v>77</v>
+      </c>
+      <c r="E32" t="s">
+        <v>61</v>
+      </c>
+      <c r="F32">
+        <v>132</v>
+      </c>
+      <c r="G32">
+        <v>129</v>
+      </c>
+      <c r="H32" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>7</v>
+      </c>
+      <c r="B33" t="s">
+        <v>53</v>
+      </c>
+      <c r="C33" t="s">
+        <v>78</v>
+      </c>
+      <c r="D33" t="s">
+        <v>79</v>
+      </c>
+      <c r="E33">
+        <v>232</v>
+      </c>
+      <c r="F33">
+        <v>169</v>
+      </c>
+      <c r="G33">
+        <v>217</v>
+      </c>
+      <c r="H33" t="s">
+        <v>238</v>
+      </c>
+      <c r="I33" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>7</v>
+      </c>
+      <c r="B34" t="s">
+        <v>47</v>
+      </c>
+      <c r="C34" t="s">
+        <v>80</v>
+      </c>
+      <c r="D34" t="s">
+        <v>81</v>
+      </c>
+      <c r="E34">
+        <v>239</v>
+      </c>
+      <c r="F34">
+        <v>270</v>
+      </c>
+      <c r="G34">
+        <v>309</v>
+      </c>
+      <c r="H34" t="s">
+        <v>237</v>
+      </c>
+      <c r="I34" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>13</v>
+      </c>
+      <c r="B35" t="s">
+        <v>47</v>
+      </c>
+      <c r="C35" t="s">
+        <v>82</v>
+      </c>
+      <c r="D35" t="s">
+        <v>83</v>
+      </c>
+      <c r="E35">
+        <v>252</v>
+      </c>
+      <c r="F35">
+        <v>252</v>
+      </c>
+      <c r="G35">
+        <v>296</v>
+      </c>
+      <c r="H35" t="s">
+        <v>241</v>
+      </c>
+      <c r="I35" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>7</v>
+      </c>
+      <c r="B36" t="s">
+        <v>47</v>
+      </c>
+      <c r="C36" t="s">
+        <v>84</v>
+      </c>
+      <c r="D36" t="s">
+        <v>85</v>
+      </c>
+      <c r="E36">
+        <v>196</v>
+      </c>
+      <c r="F36">
+        <v>168</v>
+      </c>
+      <c r="G36">
+        <v>191</v>
+      </c>
+      <c r="H36" t="s">
+        <v>241</v>
+      </c>
+      <c r="I36" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>13</v>
+      </c>
+      <c r="B37" t="s">
+        <v>47</v>
+      </c>
+      <c r="C37" t="s">
+        <v>86</v>
+      </c>
+      <c r="D37" t="s">
+        <v>87</v>
+      </c>
+      <c r="E37">
+        <v>217</v>
+      </c>
+      <c r="F37">
+        <v>209</v>
+      </c>
+      <c r="G37">
+        <v>204</v>
+      </c>
+      <c r="H37" t="s">
+        <v>242</v>
+      </c>
+      <c r="I37" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>13</v>
+      </c>
+      <c r="B38" t="s">
+        <v>47</v>
+      </c>
+      <c r="C38" t="s">
+        <v>88</v>
+      </c>
+      <c r="D38" t="s">
+        <v>89</v>
+      </c>
+      <c r="E38">
+        <v>93</v>
+      </c>
+      <c r="F38">
+        <v>132</v>
+      </c>
+      <c r="G38">
+        <v>143</v>
+      </c>
+      <c r="H38" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>7</v>
+      </c>
+      <c r="B39" t="s">
+        <v>47</v>
+      </c>
+      <c r="C39" t="s">
+        <v>90</v>
+      </c>
+      <c r="D39" t="s">
+        <v>91</v>
+      </c>
+      <c r="E39" t="s">
+        <v>61</v>
+      </c>
+      <c r="F39">
+        <v>68</v>
+      </c>
+      <c r="G39">
+        <v>96</v>
+      </c>
+      <c r="H39" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>13</v>
+      </c>
+      <c r="B40" t="s">
+        <v>47</v>
+      </c>
+      <c r="C40" t="s">
+        <v>92</v>
+      </c>
+      <c r="D40" t="s">
+        <v>93</v>
+      </c>
+      <c r="E40">
+        <v>103</v>
+      </c>
+      <c r="F40">
+        <v>107</v>
+      </c>
+      <c r="G40">
+        <v>93</v>
+      </c>
+      <c r="H40" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>7</v>
+      </c>
+      <c r="B41" t="s">
+        <v>47</v>
+      </c>
+      <c r="C41" t="s">
+        <v>94</v>
+      </c>
+      <c r="D41" t="s">
+        <v>95</v>
+      </c>
+      <c r="E41">
+        <v>102</v>
+      </c>
+      <c r="F41">
+        <v>108</v>
+      </c>
+      <c r="G41">
+        <v>103</v>
+      </c>
+      <c r="H41" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>7</v>
+      </c>
+      <c r="B42" t="s">
+        <v>53</v>
+      </c>
+      <c r="C42" t="s">
+        <v>96</v>
+      </c>
+      <c r="D42" t="s">
+        <v>97</v>
+      </c>
+      <c r="E42">
+        <v>72</v>
+      </c>
+      <c r="F42">
+        <v>58</v>
+      </c>
+      <c r="G42">
+        <v>57</v>
+      </c>
+      <c r="H42" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>13</v>
+      </c>
+      <c r="B43" t="s">
+        <v>53</v>
+      </c>
+      <c r="C43" t="s">
+        <v>98</v>
+      </c>
+      <c r="D43" t="s">
+        <v>99</v>
+      </c>
+      <c r="E43">
+        <v>42</v>
+      </c>
+      <c r="F43">
+        <v>22</v>
+      </c>
+      <c r="G43">
+        <v>27</v>
+      </c>
+      <c r="H43" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>7</v>
+      </c>
+      <c r="B44" t="s">
+        <v>53</v>
+      </c>
+      <c r="C44" t="s">
+        <v>100</v>
+      </c>
+      <c r="D44" t="s">
+        <v>101</v>
+      </c>
+      <c r="E44">
+        <v>53</v>
+      </c>
+      <c r="F44">
+        <v>35</v>
+      </c>
+      <c r="G44">
+        <v>55</v>
+      </c>
+      <c r="H44" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>13</v>
+      </c>
+      <c r="B45" t="s">
+        <v>53</v>
+      </c>
+      <c r="C45" t="s">
+        <v>102</v>
+      </c>
+      <c r="D45" t="s">
+        <v>103</v>
+      </c>
+      <c r="E45">
+        <v>41</v>
+      </c>
+      <c r="F45">
+        <v>24</v>
+      </c>
+      <c r="G45">
+        <v>33</v>
+      </c>
+      <c r="H45" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>7</v>
+      </c>
+      <c r="B46" t="s">
+        <v>53</v>
+      </c>
+      <c r="C46" t="s">
+        <v>104</v>
+      </c>
+      <c r="D46" t="s">
+        <v>105</v>
+      </c>
+      <c r="E46">
+        <v>29</v>
+      </c>
+      <c r="F46">
+        <v>23</v>
+      </c>
+      <c r="G46">
+        <v>24</v>
+      </c>
+      <c r="H46" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>13</v>
+      </c>
+      <c r="B47" t="s">
+        <v>53</v>
+      </c>
+      <c r="C47" t="s">
+        <v>106</v>
+      </c>
+      <c r="D47" t="s">
+        <v>107</v>
+      </c>
+      <c r="E47">
+        <v>3</v>
+      </c>
+      <c r="F47">
+        <v>3</v>
+      </c>
+      <c r="G47">
+        <v>3</v>
+      </c>
+      <c r="H47" t="s">
+        <v>237</v>
+      </c>
+      <c r="I47" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>13</v>
+      </c>
+      <c r="B48" t="s">
+        <v>53</v>
+      </c>
+      <c r="C48" t="s">
+        <v>108</v>
+      </c>
+      <c r="D48" t="s">
+        <v>109</v>
+      </c>
+      <c r="E48">
+        <v>39</v>
+      </c>
+      <c r="F48">
+        <v>57</v>
+      </c>
+      <c r="G48">
+        <v>56</v>
+      </c>
+      <c r="H48" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>13</v>
+      </c>
+      <c r="B49" t="s">
+        <v>47</v>
+      </c>
+      <c r="C49" t="s">
+        <v>110</v>
+      </c>
+      <c r="D49" t="s">
+        <v>111</v>
+      </c>
+      <c r="E49">
+        <v>134</v>
+      </c>
+      <c r="F49">
+        <v>130</v>
+      </c>
+      <c r="G49">
+        <v>173</v>
+      </c>
+      <c r="H49" t="s">
+        <v>236</v>
+      </c>
+      <c r="I49" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>7</v>
+      </c>
+      <c r="B50" t="s">
+        <v>47</v>
+      </c>
+      <c r="C50" t="s">
+        <v>112</v>
+      </c>
+      <c r="D50" t="s">
+        <v>113</v>
+      </c>
+      <c r="E50">
+        <v>240</v>
+      </c>
+      <c r="F50">
+        <v>248</v>
+      </c>
+      <c r="G50">
+        <v>264</v>
+      </c>
+      <c r="H50" t="s">
+        <v>236</v>
+      </c>
+      <c r="I50" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>7</v>
+      </c>
+      <c r="B51" t="s">
+        <v>47</v>
+      </c>
+      <c r="C51" t="s">
+        <v>114</v>
+      </c>
+      <c r="D51" t="s">
+        <v>115</v>
+      </c>
+      <c r="E51">
+        <v>154</v>
+      </c>
+      <c r="F51">
+        <v>128</v>
+      </c>
+      <c r="G51">
+        <v>147</v>
+      </c>
+      <c r="H51" t="s">
+        <v>249</v>
+      </c>
+      <c r="I51" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>7</v>
+      </c>
+      <c r="B52" t="s">
+        <v>53</v>
+      </c>
+      <c r="C52" t="s">
+        <v>116</v>
+      </c>
+      <c r="D52" t="s">
+        <v>117</v>
+      </c>
+      <c r="E52">
+        <v>40</v>
+      </c>
+      <c r="F52">
+        <v>41</v>
+      </c>
+      <c r="G52">
+        <v>43</v>
+      </c>
+      <c r="H52" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>7</v>
+      </c>
+      <c r="B53" t="s">
+        <v>53</v>
+      </c>
+      <c r="C53" t="s">
+        <v>118</v>
+      </c>
+      <c r="D53" t="s">
+        <v>119</v>
+      </c>
+      <c r="E53">
+        <v>21</v>
+      </c>
+      <c r="F53">
+        <v>28</v>
+      </c>
+      <c r="G53">
+        <v>33</v>
+      </c>
+      <c r="H53" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>13</v>
+      </c>
+      <c r="B54" t="s">
+        <v>47</v>
+      </c>
+      <c r="C54" t="s">
+        <v>120</v>
+      </c>
+      <c r="D54" t="s">
+        <v>121</v>
+      </c>
+      <c r="E54" t="s">
+        <v>61</v>
+      </c>
+      <c r="F54">
+        <v>110</v>
+      </c>
+      <c r="G54">
+        <v>83</v>
+      </c>
+      <c r="H54" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>52</v>
+      </c>
+      <c r="B55" t="s">
+        <v>53</v>
+      </c>
+      <c r="C55" t="s">
+        <v>122</v>
+      </c>
+      <c r="D55" t="s">
+        <v>123</v>
+      </c>
+      <c r="E55">
+        <v>14</v>
+      </c>
+      <c r="F55">
+        <v>29</v>
+      </c>
+      <c r="G55">
+        <v>44</v>
+      </c>
+      <c r="H55" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>7</v>
+      </c>
+      <c r="B56" t="s">
+        <v>124</v>
+      </c>
+      <c r="C56" t="s">
+        <v>125</v>
+      </c>
+      <c r="D56" t="s">
+        <v>126</v>
+      </c>
+      <c r="E56">
+        <v>92</v>
+      </c>
+      <c r="F56">
+        <v>65</v>
+      </c>
+      <c r="G56">
+        <v>78</v>
+      </c>
+      <c r="H56" t="s">
+        <v>246</v>
+      </c>
+      <c r="I56" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>13</v>
+      </c>
+      <c r="B57" t="s">
+        <v>124</v>
+      </c>
+      <c r="C57" t="s">
+        <v>127</v>
+      </c>
+      <c r="D57" t="s">
+        <v>128</v>
+      </c>
+      <c r="E57">
+        <v>80</v>
+      </c>
+      <c r="F57">
+        <v>71</v>
+      </c>
+      <c r="G57">
+        <v>53</v>
+      </c>
+      <c r="H57" t="s">
+        <v>240</v>
+      </c>
+      <c r="I57" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>7</v>
+      </c>
+      <c r="B58" t="s">
+        <v>124</v>
+      </c>
+      <c r="C58" t="s">
+        <v>129</v>
+      </c>
+      <c r="D58" t="s">
+        <v>51</v>
+      </c>
+      <c r="E58">
+        <v>97</v>
+      </c>
+      <c r="F58">
+        <v>62</v>
+      </c>
+      <c r="G58">
+        <v>59</v>
+      </c>
+      <c r="H58" t="s">
+        <v>250</v>
+      </c>
+      <c r="I58" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>7</v>
+      </c>
+      <c r="B59" t="s">
+        <v>58</v>
+      </c>
+      <c r="C59" t="s">
+        <v>130</v>
+      </c>
+      <c r="D59" t="s">
+        <v>131</v>
+      </c>
+      <c r="E59" t="s">
+        <v>61</v>
+      </c>
+      <c r="F59" t="s">
+        <v>61</v>
+      </c>
+      <c r="G59">
+        <v>16</v>
+      </c>
+      <c r="H59" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>7</v>
+      </c>
+      <c r="B60" t="s">
+        <v>124</v>
+      </c>
+      <c r="C60" t="s">
+        <v>132</v>
+      </c>
+      <c r="D60" t="s">
+        <v>133</v>
+      </c>
+      <c r="E60">
+        <v>37</v>
+      </c>
+      <c r="F60">
+        <v>88</v>
+      </c>
+      <c r="G60">
+        <v>70</v>
+      </c>
+      <c r="H60" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>7</v>
+      </c>
+      <c r="B61" t="s">
+        <v>124</v>
+      </c>
+      <c r="C61" t="s">
+        <v>134</v>
+      </c>
+      <c r="D61" t="s">
+        <v>135</v>
+      </c>
+      <c r="E61">
+        <v>220</v>
+      </c>
+      <c r="F61">
+        <v>180</v>
+      </c>
+      <c r="G61">
+        <v>180</v>
+      </c>
+      <c r="H61" t="s">
+        <v>238</v>
+      </c>
+      <c r="I61" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>13</v>
+      </c>
+      <c r="B62" t="s">
+        <v>58</v>
+      </c>
+      <c r="C62" t="s">
+        <v>136</v>
+      </c>
+      <c r="D62" t="s">
+        <v>137</v>
+      </c>
+      <c r="E62">
+        <v>31</v>
+      </c>
+      <c r="F62">
+        <v>28</v>
+      </c>
+      <c r="G62">
+        <v>40</v>
+      </c>
+      <c r="H62" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>13</v>
+      </c>
+      <c r="B63" t="s">
+        <v>124</v>
+      </c>
+      <c r="C63" t="s">
+        <v>138</v>
+      </c>
+      <c r="D63" t="s">
+        <v>139</v>
+      </c>
+      <c r="E63">
+        <v>84</v>
+      </c>
+      <c r="F63">
+        <v>86</v>
+      </c>
+      <c r="G63">
+        <v>54</v>
+      </c>
+      <c r="H63" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>13</v>
+      </c>
+      <c r="B64" t="s">
+        <v>124</v>
+      </c>
+      <c r="C64" t="s">
+        <v>140</v>
+      </c>
+      <c r="D64" t="s">
+        <v>141</v>
+      </c>
+      <c r="E64">
+        <v>10</v>
+      </c>
+      <c r="F64">
+        <v>26</v>
+      </c>
+      <c r="G64">
+        <v>9</v>
+      </c>
+      <c r="H64" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>13</v>
+      </c>
+      <c r="B65" t="s">
+        <v>58</v>
+      </c>
+      <c r="C65" t="s">
+        <v>142</v>
+      </c>
+      <c r="D65" t="s">
+        <v>143</v>
+      </c>
+      <c r="E65">
+        <v>31</v>
+      </c>
+      <c r="F65">
+        <v>19</v>
+      </c>
+      <c r="G65">
+        <v>22</v>
+      </c>
+      <c r="H65" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>13</v>
+      </c>
+      <c r="B66" t="s">
+        <v>58</v>
+      </c>
+      <c r="C66" t="s">
+        <v>144</v>
+      </c>
+      <c r="D66" t="s">
+        <v>145</v>
+      </c>
+      <c r="E66">
+        <v>56</v>
+      </c>
+      <c r="F66">
+        <v>65</v>
+      </c>
+      <c r="G66">
+        <v>42</v>
+      </c>
+      <c r="H66" t="s">
+        <v>237</v>
+      </c>
+      <c r="I66" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="67" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>7</v>
+      </c>
+      <c r="B67" t="s">
+        <v>58</v>
+      </c>
+      <c r="C67" t="s">
+        <v>146</v>
+      </c>
+      <c r="D67" t="s">
+        <v>147</v>
+      </c>
+      <c r="E67" t="s">
+        <v>61</v>
+      </c>
+      <c r="F67" t="s">
+        <v>61</v>
+      </c>
+      <c r="G67">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="68" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>13</v>
+      </c>
+      <c r="B68" t="s">
+        <v>58</v>
+      </c>
+      <c r="C68" t="s">
+        <v>148</v>
+      </c>
+      <c r="D68" t="s">
+        <v>149</v>
+      </c>
+      <c r="E68" t="s">
+        <v>150</v>
+      </c>
+      <c r="F68">
+        <v>10</v>
+      </c>
+      <c r="G68" t="s">
+        <v>150</v>
+      </c>
+      <c r="H68" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="69" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>13</v>
+      </c>
+      <c r="B69" t="s">
+        <v>58</v>
+      </c>
+      <c r="C69" t="s">
+        <v>151</v>
+      </c>
+      <c r="D69" t="s">
+        <v>152</v>
+      </c>
+      <c r="E69" t="s">
+        <v>61</v>
+      </c>
+      <c r="F69" t="s">
+        <v>61</v>
+      </c>
+      <c r="G69">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="70" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>13</v>
+      </c>
+      <c r="B70" t="s">
+        <v>124</v>
+      </c>
+      <c r="C70" t="s">
+        <v>153</v>
+      </c>
+      <c r="D70" t="s">
+        <v>154</v>
+      </c>
+      <c r="E70">
+        <v>46</v>
+      </c>
+      <c r="F70">
+        <v>56</v>
+      </c>
+      <c r="G70">
+        <v>24</v>
+      </c>
+      <c r="H70" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="71" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>13</v>
+      </c>
+      <c r="B71" t="s">
+        <v>124</v>
+      </c>
+      <c r="C71" t="s">
+        <v>155</v>
+      </c>
+      <c r="D71" t="s">
+        <v>156</v>
+      </c>
+      <c r="E71">
+        <v>139</v>
+      </c>
+      <c r="F71">
+        <v>164</v>
+      </c>
+      <c r="G71">
+        <v>151</v>
+      </c>
+      <c r="H71" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="72" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>13</v>
+      </c>
+      <c r="B72" t="s">
+        <v>124</v>
+      </c>
+      <c r="C72" t="s">
+        <v>157</v>
+      </c>
+      <c r="D72" t="s">
+        <v>158</v>
+      </c>
+      <c r="E72">
+        <v>18</v>
+      </c>
+      <c r="F72">
+        <v>34</v>
+      </c>
+      <c r="G72">
+        <v>29</v>
+      </c>
+      <c r="H72" t="s">
+        <v>243</v>
+      </c>
+      <c r="I72" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="73" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>7</v>
+      </c>
+      <c r="B73" t="s">
+        <v>124</v>
+      </c>
+      <c r="C73" t="s">
+        <v>159</v>
+      </c>
+      <c r="D73" t="s">
+        <v>160</v>
+      </c>
+      <c r="E73">
+        <v>86</v>
+      </c>
+      <c r="F73">
+        <v>110</v>
+      </c>
+      <c r="G73">
+        <v>81</v>
+      </c>
+      <c r="H73" t="s">
+        <v>240</v>
+      </c>
+      <c r="I73" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="74" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>7</v>
+      </c>
+      <c r="B74" t="s">
+        <v>124</v>
+      </c>
+      <c r="C74" t="s">
+        <v>161</v>
+      </c>
+      <c r="D74" t="s">
+        <v>162</v>
+      </c>
+      <c r="E74">
+        <v>87</v>
+      </c>
+      <c r="F74">
+        <v>111</v>
+      </c>
+      <c r="G74">
+        <v>79</v>
+      </c>
+      <c r="H74" t="s">
+        <v>243</v>
+      </c>
+      <c r="I74" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="75" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>13</v>
+      </c>
+      <c r="B75" t="s">
+        <v>124</v>
+      </c>
+      <c r="C75" t="s">
+        <v>163</v>
+      </c>
+      <c r="D75" t="s">
+        <v>164</v>
+      </c>
+      <c r="E75">
+        <v>33</v>
+      </c>
+      <c r="F75">
+        <v>46</v>
+      </c>
+      <c r="G75">
+        <v>36</v>
+      </c>
+      <c r="H75" t="s">
+        <v>240</v>
+      </c>
+      <c r="I75" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="76" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>13</v>
+      </c>
+      <c r="B76" t="s">
+        <v>124</v>
+      </c>
+      <c r="C76" t="s">
+        <v>165</v>
+      </c>
+      <c r="D76" t="s">
+        <v>166</v>
+      </c>
+      <c r="E76">
+        <v>108</v>
+      </c>
+      <c r="F76">
+        <v>114</v>
+      </c>
+      <c r="G76">
+        <v>69</v>
+      </c>
+      <c r="H76" t="s">
+        <v>253</v>
+      </c>
+      <c r="I76" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="77" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
+        <v>13</v>
+      </c>
+      <c r="B77" t="s">
+        <v>124</v>
+      </c>
+      <c r="C77" t="s">
+        <v>167</v>
+      </c>
+      <c r="D77" t="s">
+        <v>168</v>
+      </c>
+      <c r="E77">
+        <v>110</v>
+      </c>
+      <c r="F77">
+        <v>96</v>
+      </c>
+      <c r="G77">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="78" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
+        <v>13</v>
+      </c>
+      <c r="B78" t="s">
+        <v>124</v>
+      </c>
+      <c r="C78" t="s">
+        <v>169</v>
+      </c>
+      <c r="D78" t="s">
+        <v>170</v>
+      </c>
+      <c r="E78">
+        <v>111</v>
+      </c>
+      <c r="F78">
+        <v>144</v>
+      </c>
+      <c r="G78">
+        <v>123</v>
+      </c>
+      <c r="H78" t="s">
+        <v>236</v>
+      </c>
+      <c r="I78" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="79" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
+        <v>7</v>
+      </c>
+      <c r="B79" t="s">
+        <v>124</v>
+      </c>
+      <c r="C79" t="s">
+        <v>171</v>
+      </c>
+      <c r="D79" t="s">
+        <v>172</v>
+      </c>
+      <c r="E79">
+        <v>158</v>
+      </c>
+      <c r="F79">
+        <v>165</v>
+      </c>
+      <c r="G79">
+        <v>139</v>
+      </c>
+      <c r="H79" t="s">
+        <v>236</v>
+      </c>
+      <c r="I79" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="80" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
+        <v>7</v>
+      </c>
+      <c r="B80" t="s">
+        <v>124</v>
+      </c>
+      <c r="C80" t="s">
+        <v>173</v>
+      </c>
+      <c r="D80" t="s">
+        <v>174</v>
+      </c>
+      <c r="E80">
+        <v>161</v>
+      </c>
+      <c r="F80">
+        <v>196</v>
+      </c>
+      <c r="G80">
+        <v>162</v>
+      </c>
+      <c r="H80" t="s">
+        <v>236</v>
+      </c>
+      <c r="I80" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="81" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
+        <v>7</v>
+      </c>
+      <c r="B81" t="s">
+        <v>58</v>
+      </c>
+      <c r="C81" t="s">
+        <v>175</v>
+      </c>
+      <c r="D81" t="s">
+        <v>176</v>
+      </c>
+      <c r="E81" t="s">
+        <v>61</v>
+      </c>
+      <c r="F81">
+        <v>48</v>
+      </c>
+      <c r="G81" t="s">
+        <v>61</v>
+      </c>
+      <c r="H81" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="82" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
+        <v>7</v>
+      </c>
+      <c r="B82" t="s">
+        <v>58</v>
+      </c>
+      <c r="C82" t="s">
+        <v>177</v>
+      </c>
+      <c r="D82" t="s">
+        <v>178</v>
+      </c>
+      <c r="E82">
+        <v>39</v>
+      </c>
+      <c r="F82" t="s">
+        <v>61</v>
+      </c>
+      <c r="G82">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="83" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
+        <v>13</v>
+      </c>
+      <c r="B83" t="s">
+        <v>58</v>
+      </c>
+      <c r="C83" t="s">
+        <v>179</v>
+      </c>
+      <c r="D83" t="s">
+        <v>180</v>
+      </c>
+      <c r="E83" t="s">
+        <v>61</v>
+      </c>
+      <c r="F83">
+        <v>78</v>
+      </c>
+      <c r="G83" t="s">
+        <v>61</v>
+      </c>
+      <c r="H83" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="84" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
+        <v>13</v>
+      </c>
+      <c r="B84" t="s">
+        <v>58</v>
+      </c>
+      <c r="C84" t="s">
+        <v>181</v>
+      </c>
+      <c r="D84" t="s">
+        <v>182</v>
+      </c>
+      <c r="E84">
+        <v>25</v>
+      </c>
+      <c r="F84" t="s">
+        <v>61</v>
+      </c>
+      <c r="G84">
+        <v>79</v>
+      </c>
+      <c r="I84" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="85" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
+        <v>13</v>
+      </c>
+      <c r="B85" t="s">
+        <v>124</v>
+      </c>
+      <c r="C85" t="s">
+        <v>183</v>
+      </c>
+      <c r="D85" t="s">
+        <v>184</v>
+      </c>
+      <c r="E85">
+        <v>65</v>
+      </c>
+      <c r="F85">
+        <v>51</v>
+      </c>
+      <c r="G85">
+        <v>48</v>
+      </c>
+      <c r="H85" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="86" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A86" t="s">
+        <v>13</v>
+      </c>
+      <c r="B86" t="s">
+        <v>124</v>
+      </c>
+      <c r="C86" t="s">
+        <v>185</v>
+      </c>
+      <c r="D86" t="s">
+        <v>186</v>
+      </c>
+      <c r="E86">
+        <v>124</v>
+      </c>
+      <c r="F86">
+        <v>178</v>
+      </c>
+      <c r="G86">
+        <v>186</v>
+      </c>
+      <c r="H86" t="s">
+        <v>236</v>
+      </c>
+      <c r="I86" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="87" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A87" t="s">
+        <v>7</v>
+      </c>
+      <c r="B87" t="s">
+        <v>124</v>
+      </c>
+      <c r="C87" t="s">
+        <v>187</v>
+      </c>
+      <c r="D87" t="s">
+        <v>188</v>
+      </c>
+      <c r="E87">
+        <v>150</v>
+      </c>
+      <c r="F87">
+        <v>141</v>
+      </c>
+      <c r="G87">
+        <v>140</v>
+      </c>
+      <c r="H87" t="s">
+        <v>236</v>
+      </c>
+      <c r="I87" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="88" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A88" t="s">
+        <v>13</v>
+      </c>
+      <c r="B88" t="s">
+        <v>124</v>
+      </c>
+      <c r="C88" t="s">
+        <v>189</v>
+      </c>
+      <c r="D88" t="s">
+        <v>190</v>
+      </c>
+      <c r="E88">
+        <v>105</v>
+      </c>
+      <c r="F88">
+        <v>125</v>
+      </c>
+      <c r="G88">
+        <v>97</v>
+      </c>
+      <c r="H88" t="s">
+        <v>236</v>
+      </c>
+      <c r="I88" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="89" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A89" t="s">
+        <v>13</v>
+      </c>
+      <c r="B89" t="s">
+        <v>124</v>
+      </c>
+      <c r="C89" t="s">
+        <v>191</v>
+      </c>
+      <c r="D89" t="s">
+        <v>192</v>
+      </c>
+      <c r="E89" t="s">
+        <v>61</v>
+      </c>
+      <c r="F89">
+        <v>41</v>
+      </c>
+      <c r="G89">
+        <v>38</v>
+      </c>
+      <c r="H89" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="90" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A90" t="s">
+        <v>13</v>
+      </c>
+      <c r="B90" t="s">
+        <v>124</v>
+      </c>
+      <c r="C90" t="s">
+        <v>193</v>
+      </c>
+      <c r="D90" t="s">
+        <v>194</v>
+      </c>
+      <c r="E90">
+        <v>65</v>
+      </c>
+      <c r="F90">
+        <v>55</v>
+      </c>
+      <c r="G90">
+        <v>72</v>
+      </c>
+      <c r="H90" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="91" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A91" t="s">
+        <v>13</v>
+      </c>
+      <c r="B91" t="s">
+        <v>124</v>
+      </c>
+      <c r="C91" t="s">
+        <v>195</v>
+      </c>
+      <c r="D91" t="s">
+        <v>196</v>
+      </c>
+      <c r="E91">
+        <v>33</v>
+      </c>
+      <c r="F91">
+        <v>17</v>
+      </c>
+      <c r="G91">
+        <v>19</v>
+      </c>
+      <c r="H91" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="92" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A92" t="s">
+        <v>52</v>
+      </c>
+      <c r="B92" t="s">
+        <v>124</v>
+      </c>
+      <c r="C92" t="s">
+        <v>197</v>
+      </c>
+      <c r="D92" t="s">
+        <v>198</v>
+      </c>
+      <c r="E92">
+        <v>35</v>
+      </c>
+      <c r="F92">
+        <v>30</v>
+      </c>
+      <c r="G92">
+        <v>22</v>
+      </c>
+      <c r="H92" t="s">
+        <v>237</v>
+      </c>
+      <c r="I92" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="93" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A93" t="s">
+        <v>7</v>
+      </c>
+      <c r="B93" t="s">
+        <v>124</v>
+      </c>
+      <c r="C93" t="s">
+        <v>199</v>
+      </c>
+      <c r="D93" t="s">
+        <v>200</v>
+      </c>
+      <c r="E93">
+        <v>269</v>
+      </c>
+      <c r="F93">
+        <v>265</v>
+      </c>
+      <c r="G93">
+        <v>229</v>
+      </c>
+      <c r="H93" t="s">
+        <v>255</v>
+      </c>
+      <c r="I93" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="94" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A94" t="s">
+        <v>13</v>
+      </c>
+      <c r="B94" t="s">
+        <v>124</v>
+      </c>
+      <c r="C94" t="s">
+        <v>201</v>
+      </c>
+      <c r="D94" t="s">
+        <v>202</v>
+      </c>
+      <c r="E94">
+        <v>38</v>
+      </c>
+      <c r="F94">
+        <v>57</v>
+      </c>
+      <c r="G94">
+        <v>39</v>
+      </c>
+      <c r="H94" t="s">
+        <v>243</v>
+      </c>
+      <c r="I94" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="95" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A95" t="s">
+        <v>7</v>
+      </c>
+      <c r="B95" t="s">
+        <v>124</v>
+      </c>
+      <c r="C95" t="s">
+        <v>203</v>
+      </c>
+      <c r="D95" t="s">
+        <v>204</v>
+      </c>
+      <c r="E95">
+        <v>25</v>
+      </c>
+      <c r="F95">
+        <v>17</v>
+      </c>
+      <c r="G95">
+        <v>23</v>
+      </c>
+      <c r="H95" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="96" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A96" t="s">
+        <v>13</v>
+      </c>
+      <c r="B96" t="s">
+        <v>124</v>
+      </c>
+      <c r="C96" t="s">
+        <v>205</v>
+      </c>
+      <c r="D96" t="s">
+        <v>206</v>
+      </c>
+      <c r="E96">
+        <v>30</v>
+      </c>
+      <c r="F96">
+        <v>29</v>
+      </c>
+      <c r="G96">
+        <v>28</v>
+      </c>
+      <c r="H96" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="97" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A97" t="s">
+        <v>13</v>
+      </c>
+      <c r="B97" t="s">
+        <v>124</v>
+      </c>
+      <c r="C97" t="s">
+        <v>207</v>
+      </c>
+      <c r="D97" t="s">
+        <v>208</v>
+      </c>
+      <c r="E97">
+        <v>184</v>
+      </c>
+      <c r="F97">
+        <v>209</v>
+      </c>
+      <c r="G97">
+        <v>163</v>
+      </c>
+      <c r="H97" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="98" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A98" t="s">
+        <v>13</v>
+      </c>
+      <c r="B98" t="s">
+        <v>58</v>
+      </c>
+      <c r="C98" t="s">
+        <v>209</v>
+      </c>
+      <c r="D98" t="s">
+        <v>210</v>
+      </c>
+      <c r="E98">
+        <v>18</v>
+      </c>
+      <c r="F98">
+        <v>17</v>
+      </c>
+      <c r="G98">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="99" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A99" t="s">
+        <v>13</v>
+      </c>
+      <c r="B99" t="s">
+        <v>58</v>
+      </c>
+      <c r="C99" t="s">
+        <v>211</v>
+      </c>
+      <c r="D99" t="s">
+        <v>212</v>
+      </c>
+      <c r="E99">
+        <v>58</v>
+      </c>
+      <c r="F99">
+        <v>69</v>
+      </c>
+      <c r="G99">
+        <v>49</v>
+      </c>
+      <c r="H99" t="s">
+        <v>237</v>
+      </c>
+      <c r="I99" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="100" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A100" t="s">
+        <v>7</v>
+      </c>
+      <c r="B100" t="s">
+        <v>58</v>
+      </c>
+      <c r="C100" t="s">
+        <v>213</v>
+      </c>
+      <c r="D100" t="s">
+        <v>214</v>
+      </c>
+      <c r="E100">
+        <v>33</v>
+      </c>
+      <c r="F100">
+        <v>35</v>
+      </c>
+      <c r="G100">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="101" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A101" t="s">
+        <v>13</v>
+      </c>
+      <c r="B101" t="s">
+        <v>58</v>
+      </c>
+      <c r="C101" t="s">
+        <v>215</v>
+      </c>
+      <c r="D101" t="s">
+        <v>216</v>
+      </c>
+      <c r="E101">
+        <v>23</v>
+      </c>
+      <c r="F101" t="s">
+        <v>61</v>
+      </c>
+      <c r="G101">
+        <v>19</v>
+      </c>
+      <c r="H101" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="102" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A102" t="s">
+        <v>13</v>
+      </c>
+      <c r="B102" t="s">
+        <v>58</v>
+      </c>
+      <c r="C102" t="s">
+        <v>217</v>
+      </c>
+      <c r="D102" t="s">
+        <v>218</v>
+      </c>
+      <c r="E102" t="s">
+        <v>61</v>
+      </c>
+      <c r="F102">
+        <v>14</v>
+      </c>
+      <c r="G102" t="s">
+        <v>61</v>
+      </c>
+      <c r="H102" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="103" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A103" t="s">
+        <v>13</v>
+      </c>
+      <c r="B103" t="s">
+        <v>124</v>
+      </c>
+      <c r="C103" t="s">
+        <v>219</v>
+      </c>
+      <c r="D103" t="s">
+        <v>220</v>
+      </c>
+      <c r="E103">
+        <v>34</v>
+      </c>
+      <c r="F103">
+        <v>43</v>
+      </c>
+      <c r="G103">
+        <v>36</v>
+      </c>
+      <c r="H103" t="s">
+        <v>257</v>
+      </c>
+      <c r="I103" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="104" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A104" t="s">
+        <v>7</v>
+      </c>
+      <c r="B104" t="s">
+        <v>124</v>
+      </c>
+      <c r="C104" t="s">
+        <v>221</v>
+      </c>
+      <c r="D104" t="s">
+        <v>222</v>
+      </c>
+      <c r="E104" t="s">
+        <v>61</v>
+      </c>
+      <c r="F104">
+        <v>37</v>
+      </c>
+      <c r="G104">
+        <v>48</v>
+      </c>
+      <c r="H104" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="105" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A105" t="s">
+        <v>7</v>
+      </c>
+      <c r="B105" t="s">
+        <v>124</v>
+      </c>
+      <c r="C105" t="s">
+        <v>223</v>
+      </c>
+      <c r="D105" t="s">
+        <v>224</v>
+      </c>
+      <c r="E105" t="s">
+        <v>61</v>
+      </c>
+      <c r="F105">
+        <v>19</v>
+      </c>
+      <c r="G105">
+        <v>31</v>
+      </c>
+      <c r="H105" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="106" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A106" t="s">
+        <v>13</v>
+      </c>
+      <c r="B106" t="s">
+        <v>58</v>
+      </c>
+      <c r="C106" t="s">
+        <v>225</v>
+      </c>
+      <c r="D106" t="s">
+        <v>226</v>
+      </c>
+      <c r="E106" t="s">
+        <v>61</v>
+      </c>
+      <c r="F106" t="s">
+        <v>61</v>
+      </c>
+      <c r="G106">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="107" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A107" t="s">
+        <v>7</v>
+      </c>
+      <c r="B107" t="s">
+        <v>58</v>
+      </c>
+      <c r="C107" t="s">
+        <v>227</v>
+      </c>
+      <c r="D107" t="s">
+        <v>228</v>
+      </c>
+      <c r="E107" t="s">
+        <v>61</v>
+      </c>
+      <c r="F107" t="s">
+        <v>61</v>
+      </c>
+      <c r="G107">
+        <v>38</v>
+      </c>
+      <c r="H107" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="108" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A108" t="s">
+        <v>7</v>
+      </c>
+      <c r="B108" t="s">
+        <v>58</v>
+      </c>
+      <c r="C108" t="s">
+        <v>229</v>
+      </c>
+      <c r="D108" t="s">
+        <v>230</v>
+      </c>
+      <c r="E108" t="s">
+        <v>61</v>
+      </c>
+      <c r="F108" t="s">
+        <v>61</v>
+      </c>
+      <c r="G108">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="109" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A109" t="s">
+        <v>13</v>
+      </c>
+      <c r="B109" t="s">
+        <v>124</v>
+      </c>
+      <c r="C109" t="s">
+        <v>231</v>
+      </c>
+      <c r="D109" t="s">
+        <v>232</v>
+      </c>
+      <c r="E109" t="s">
+        <v>61</v>
+      </c>
+      <c r="F109" t="s">
+        <v>61</v>
+      </c>
+      <c r="G109">
+        <v>11</v>
+      </c>
+      <c r="H109" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="110" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A110" t="s">
+        <v>13</v>
+      </c>
+      <c r="B110" t="s">
+        <v>124</v>
+      </c>
+      <c r="C110" t="s">
+        <v>233</v>
+      </c>
+      <c r="D110" t="s">
+        <v>234</v>
+      </c>
+      <c r="E110" t="s">
+        <v>61</v>
+      </c>
+      <c r="F110" t="s">
+        <v>61</v>
+      </c>
+      <c r="G110">
+        <v>19</v>
+      </c>
+      <c r="H110" t="s">
+        <v>237</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100347DA14A51159347908FCB644918D075" ma:contentTypeVersion="4" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="f74c0c6907a9c4c0d2bc11040657d8f6">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="b2471f7f-c541-44b1-a67d-1fdff98d7327" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="c15f0e2457fdefd102a89a6f1db48816" ns2:_="">
     <xsd:import namespace="b2471f7f-c541-44b1-a67d-1fdff98d7327"/>
@@ -3812,10 +6949,37 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3DE78B51-7529-42A0-9419-7953144BB158}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{917A63A9-924A-4433-A5CA-15E6D539A175}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="b2471f7f-c541-44b1-a67d-1fdff98d7327"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{917A63A9-924A-4433-A5CA-15E6D539A175}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3DE78B51-7529-42A0-9419-7953144BB158}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
added workshop groups for the timetable data
</commit_message>
<xml_diff>
--- a/Raw Data/Course Enrollment Numbers.xlsx
+++ b/Raw Data/Course Enrollment Numbers.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uoe-my.sharepoint.com/personal/s1941220_ed_ac_uk/Documents/Year 5/SEM2/Topics in Applied OR/taor_project/taor_project/Raw Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="4" documentId="11_883825DC4981F6E10CE451C5E8584356D790E938" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{86C5821A-BFB3-4300-81B0-5C0EEC9AE058}"/>
+  <xr:revisionPtr revIDLastSave="6" documentId="11_883825DC4981F6E10CE451C5E8584356D790E938" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{73CD9062-6F90-4949-9300-868A6F10D582}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Course Numbers" sheetId="1" r:id="rId1"/>
@@ -7196,8 +7196,8 @@
   </sheetPr>
   <dimension ref="A1:N110"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A81" zoomScale="70" workbookViewId="0">
-      <selection activeCell="M88" sqref="M88"/>
+    <sheetView tabSelected="1" topLeftCell="A80" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="H103" sqref="H103"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7208,7 +7208,8 @@
     <col min="4" max="4" width="49.5546875" bestFit="1" customWidth="1"/>
     <col min="5" max="6" width="13.5546875" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="13.5546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="13.5546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="74.109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.5546875" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="24.5546875" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="62.21875" bestFit="1" customWidth="1"/>
     <col min="12" max="13" width="13.5546875" bestFit="1" customWidth="1"/>
@@ -10677,7 +10678,7 @@
         <v>36</v>
       </c>
       <c r="H103" t="s">
-        <v>376</v>
+        <v>82</v>
       </c>
       <c r="I103" t="s">
         <v>274</v>

</xml_diff>